<commit_message>
Progetto linguaggi a, iniziata relazione
</commit_message>
<xml_diff>
--- a/Bruniera/linguaggi e compilatori/progetto/parteA/run.xlsx
+++ b/Bruniera/linguaggi e compilatori/progetto/parteA/run.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>$P</t>
   </si>
@@ -27,6 +27,9 @@
     <t>$P'P(</t>
   </si>
   <si>
+    <t>acc</t>
+  </si>
+  <si>
     <t>$P'P</t>
   </si>
   <si>
@@ -310,16 +313,25 @@
   </si>
   <si>
     <t>$</t>
+  </si>
+  <si>
+    <t>halt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -376,25 +388,26 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,7 +915,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -932,14 +945,16 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -947,276 +962,296 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>17</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="6" t="s">
         <v>49</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
@@ -1224,300 +1259,322 @@
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25">
-      <c r="A33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>57</v>
+      <c r="B33" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="1"/>
+      <c r="A35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="C36" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>63</v>
+      <c r="A37" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="1"/>
+      <c r="A39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="8" t="s">
         <v>69</v>
       </c>
+      <c r="B40" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="8" t="s">
         <v>73</v>
       </c>
+      <c r="B42" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="C42" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" ht="14.25">
       <c r="A44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" ht="14.25">
       <c r="A45" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="8" t="s">
         <v>77</v>
       </c>
+      <c r="B45" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="C45" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" ht="14.25">
       <c r="A46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" ht="14.25">
       <c r="A47" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" ht="14.25">
       <c r="A48" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="8" t="s">
         <v>83</v>
       </c>
+      <c r="B49" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="C49" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" ht="14.25">
       <c r="A50" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" ht="14.25">
       <c r="A51" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" ht="14.25">
       <c r="A53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>90</v>
+      <c r="C53" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="54" ht="14.25">
       <c r="A54" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="55" ht="14.25">
       <c r="A55" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="6" t="s">
         <v>93</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="56" ht="14.25">
       <c r="A56" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" ht="14.25">
       <c r="A57" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C57" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" ht="14.25">
       <c r="A58" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" ht="14.25">
       <c r="A59" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C59" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>